<commit_message>
Sorting files and folder
</commit_message>
<xml_diff>
--- a/Datasets/3. Base de Indicadores de Turismo.xlsx
+++ b/Datasets/3. Base de Indicadores de Turismo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\IDT\correlation\Bases_Datos_DS4A_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8a998fd753787cc/Documents/DS4A Colombia Cohort 6/Project_DS4A_IDT/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59638601-9956-43E4-9B00-C822F90F33F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{59638601-9956-43E4-9B00-C822F90F33F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0857B7C3-7DD6-47BB-AB18-BE9E77FB67A4}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -205,18 +205,18 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,12 +513,12 @@
   <dimension ref="A1:H263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B272" sqref="B272"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -529,7 +529,7 @@
     <col min="8" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -555,7 +555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0.61143939709768602</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0.182</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -618,7 +618,7 @@
         <v>0.62825551238601196</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -641,7 +641,7 @@
         <v>0.187</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -661,7 +661,7 @@
         <v>0.585851160492046</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -684,7 +684,7 @@
         <v>0.191</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -704,7 +704,7 @@
         <v>0.58156737945425696</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -727,7 +727,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -747,7 +747,7 @@
         <v>0.58760000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -770,7 +770,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,7 +813,7 @@
         <v>0.57441666666666702</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -853,7 +853,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -876,7 +876,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0.55461666666666698</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -913,7 +913,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -936,7 +936,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -959,7 +959,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0.58309999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -996,7 +996,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0.59691666666666698</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0.62326666666666697</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>0.34899999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0.18757554032170859</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>0.52764524708586424</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0.73467228429887521</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>0.59127043266450308</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>0.69109858964003512</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>0.62613336013573828</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>0.66527449602085231</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>0.68085123501973455</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>0.67368592564236862</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>0.68490189948992641</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>0.70498350637753404</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0.66608938968512876</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>0.46970217572380502</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.47164265676350736</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>0.653820226770644</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0.62700612518083187</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>0.53793248419938344</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>0.55817678067700982</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>0.59919714323423623</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>0.6200811414754267</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>0.63522470770540418</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>0.66021391697909271</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0.65714914595683893</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>0.67865516794636249</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0.48020182438709424</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>0.48204752183259447</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>0.66851594978555429</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0.65993581296899628</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0.60820973357828823</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>0.59016057684108347</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>0.6067909466220468</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>0.60769179748140034</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0.6411894425949195</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>0.64748648108666196</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0.63713436513789534</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0.69819020038149682</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0.48991993686130125</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0.4956777952817415</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>0.66369230898464515</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0.66736944581901836</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>0.55880753814187589</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0.69885509138807289</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0.65607974123531265</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0.63674876081470788</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>0.67594931918555634</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>0.66173747921991988</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>0.63947516289371342</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0.70549524647585782</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>0.47917825919172208</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>0.4792481470065782</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0.65917294463176612</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>0.62829263214514286</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>0.55874853229773025</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.62143663789002535</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0.59462817851835603</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0.55183721957717857</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0.58417964541021639</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0.62593545917640203</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>5</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>0.63641464295790096</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0.62657537673260766</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>5</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0.46374450956064511</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>0.45252610848260871</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>5</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>0.64179148834997624</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0.55596212115572163</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>0.61227968235521979</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.57280814787312262</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0.56223883457926016</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>0.61933983495873968</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>5</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0.54783984513150796</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0.62763850201176108</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>0.65290411835146933</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0.67542811171129757</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>0.45805175849039614</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>0.46829419596925498</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>5</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>0.64239999999999997</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>0.5909717846390814</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0.53350966047645842</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.60150000000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>0.55481012180865108</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>0.58844589333663211</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>0.58404614786961906</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>0.63164173379363253</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>0.67362659711493522</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>5</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>0.6589270809621367</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.44245395071736959</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>0.45679999999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0.64190000000000003</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>5</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>0.60170000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>5</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>0.56379999999999997</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>0.58960000000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>5</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>0.54549999999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>0.59709999999999996</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>5</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>0.58350000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>5</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>0.61780000000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>0.62519999999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>0.6391</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>0.43099999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>5</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>0.44340000000000002</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>0.60829999999999995</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>0.57030000000000003</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>5</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0.55889999999999995</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>0.51539999999999997</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>0.54610000000000003</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>5</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>0.53139999999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>0.5716</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>5</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>0.61180000000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>5</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>0.66879999999999995</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>5</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>0.4214</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>0.44950000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>5</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>0.59570000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>5</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0.50749999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>5</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>0.61019999999999996</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>5</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>0.55720000000000003</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>5</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>0.56589999999999996</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>5</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>0.60619999999999996</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>5</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>0.64329999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>5</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>0.68279999999999996</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>5</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>5</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>0.47289999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>5</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>5</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>0.65029999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>5</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>0.58430000000000004</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>5</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>0.62370000000000003</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>5</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>0.59030000000000005</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>5</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>0.56740000000000002</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>5</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>0.60219999999999996</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>5</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0.63329999999999997</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>5</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>0.64200000000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>5</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>0.72450000000000003</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>5</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>5</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>0.4844</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>5</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0.66779999999999995</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>5</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>0.63370000000000004</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>5</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>0.58109999999999995</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>5</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>0.6522</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>5</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>0.60540000000000005</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>5</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>0.64449999999999996</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>5</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>0.63149999999999995</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>5</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0.67689999999999995</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>5</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>0.6653</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>5</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>0.71650000000000003</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>5</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>0.51990000000000003</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>5</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>0.52459999999999996</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>5</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>0.67779999999999996</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>5</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>0.33229999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>5</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>5</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>5.5199999999999999E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>5</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>5</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>5.5500000000000001E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>5</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>5</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>0.2021</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>5</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>0.15290000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>5</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>0.22639999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>5</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>0.24060000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>5</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>5</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>0.22270000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>5</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>0.2555</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>5</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>0.2271</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>5</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>0.22869999999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>5</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>0.2979</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>5</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>0.3488</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>5</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>0.39340000000000003</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>5</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>0.44950000000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>5</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>0.49930000000000002</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>5</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>0.58350000000000002</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>5</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>0.47720000000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>8</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>0.40180486061472481</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>8</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>0.4477332028701892</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>8</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>0.44979310344827589</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>8</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>0.44546691724450782</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>8</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>0.36086736415794801</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>8</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>0.36667479873139791</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>8</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>0.44187880153187653</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>8</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>0.38392975334245244</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>8</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>0.39918360748494525</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>8</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>0.43013381941048329</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>8</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>0.41263014166239975</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>8</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>0.40084015034269288</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>8</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>0.36857084773327914</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>8</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>0.3736691106152375</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>8</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>0.39090999950027483</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>8</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>0.37775797282975238</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>8</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>0.39308681672025725</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>8</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>0.37843471244789101</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>8</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>0.41007826928150559</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>8</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>0.39991032486854439</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>8</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>0.39759732870707182</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>8</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>0.45416222932197375</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>8</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>0.40838593484988894</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>8</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>0.41007897705904478</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>8</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>0.38225913854133808</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>8</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>0.40681739025091995</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>8</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>0.44681646939375319</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>8</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>0.48124651137462049</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>8</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>0.46262460667918243</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>8</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>0.45641991404703269</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>8</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>0.47421242684597187</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>8</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>0.45200895169812882</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>8</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>0.44152385726369875</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>8</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>0.47752188323276962</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>8</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>0.472412994829848</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>8</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>0.4470288624787776</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>8</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>0.37032160822271054</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>8</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>0.44194355126831009</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>8</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>0.46522189233533867</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>8</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>0.48189748201438848</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>8</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>0.47395160758217003</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>8</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>0.47113043338503202</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>8</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>0.47624279987295154</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>8</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>0.44072879448267527</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>8</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>0.4249215175923845</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>8</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>0.45516844273595769</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>39</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>39</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>39</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>39</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>39</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>39</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>39</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>39</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>39</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>39</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>39</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>39</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>39</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>